<commit_message>
beres tombol CRUD tapi belum fungsi, beres layout
</commit_message>
<xml_diff>
--- a/data/monalisa_sjb_arsip.xlsx
+++ b/data/monalisa_sjb_arsip.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="23">
   <si>
     <t>kpknl</t>
   </si>
@@ -60,6 +60,9 @@
     <t>KPKNL Jambi</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>KPKNL Palembang</t>
   </si>
   <si>
@@ -67,6 +70,9 @@
   </si>
   <si>
     <t>KPKNL Pangkal Pinang</t>
+  </si>
+  <si>
+    <t>Pejabat Lelang Kelas II</t>
   </si>
   <si>
     <t>pokok_q1</t>
@@ -92,24 +98,18 @@
   <si>
     <t>pnbp_q4</t>
   </si>
-  <si>
-    <t>Pejabat Lelang Kelas II</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="7">
+  <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,11 +274,6 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -597,7 +592,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -743,17 +738,14 @@
     <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -803,8 +795,6 @@
     <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
-    <cellStyle name="Comma 2" xfId="49"/>
-    <cellStyle name="Comma 2 3" xfId="50"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1107,19 +1097,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="20.6363636363636" customWidth="1"/>
-    <col min="6" max="6" width="18.3636363636364"/>
-    <col min="7" max="7" width="17.1818181818182"/>
-    <col min="8" max="9" width="15.5454545454545"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
@@ -1166,17 +1150,17 @@
       <c r="E2">
         <v>187</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>28436387900</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>1048182978</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>567411775</v>
       </c>
-      <c r="I2" s="2">
-        <v>0</v>
+      <c r="I2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1195,16 +1179,16 @@
       <c r="E3">
         <v>131</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>8774078570</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>260932373</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <v>64840375</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3">
         <v>918481182</v>
       </c>
     </row>
@@ -1224,16 +1208,16 @@
       <c r="E4">
         <v>279</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <v>22744381408</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>687374956</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4">
         <v>222773463</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4">
         <v>115191249</v>
       </c>
     </row>
@@ -1253,16 +1237,16 @@
       <c r="E5">
         <v>191</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <v>15850619013</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>489872355</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <v>193480693</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5">
         <v>164303200</v>
       </c>
     </row>
@@ -1282,22 +1266,22 @@
       <c r="E6">
         <v>168</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6">
         <v>9284728199</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>295239561</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6">
         <v>96138250</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6">
         <v>106771995</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>2025</v>
@@ -1311,22 +1295,22 @@
       <c r="E7">
         <v>99</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7">
         <v>20471496109</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7">
         <v>922321034</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7">
         <v>367583115</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7">
         <v>697666230</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>2025</v>
@@ -1340,22 +1324,22 @@
       <c r="E8">
         <v>115</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8">
         <v>13782029501</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8">
         <v>435251854</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8">
         <v>86296257.5</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8">
         <v>122230565</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>2025</v>
@@ -1369,22 +1353,22 @@
       <c r="E9">
         <v>126</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9">
         <v>18793350488</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9">
         <v>522735209</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9">
         <v>111960250</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9">
         <v>167920500</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>2025</v>
@@ -1398,22 +1382,22 @@
       <c r="E10">
         <v>123</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10">
         <v>15757602878</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10">
         <v>572865367</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10">
         <v>281172510</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10">
         <v>498345020</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>2025</v>
@@ -1427,22 +1411,22 @@
       <c r="E11">
         <v>168</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11">
         <v>23397422689</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11">
         <v>751880985</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11">
         <v>276898575</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11">
         <v>461767150</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>2025</v>
@@ -1456,22 +1440,22 @@
       <c r="E12">
         <v>24</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12">
         <v>172604700</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12">
         <v>9952094</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12">
         <v>3250000</v>
       </c>
-      <c r="I12" s="2">
-        <v>0</v>
+      <c r="I12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>2025</v>
@@ -1485,22 +1469,22 @@
       <c r="E13">
         <v>85</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13">
         <v>2978835200</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13">
         <v>79557704</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13">
         <v>13413750</v>
       </c>
-      <c r="I13" s="2">
-        <v>0</v>
+      <c r="I13" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>2025</v>
@@ -1514,22 +1498,22 @@
       <c r="E14">
         <v>141</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14">
         <v>7323407755</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14">
         <v>206085656</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14">
         <v>28592500</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14">
         <v>11325000</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>2025</v>
@@ -1543,22 +1527,22 @@
       <c r="E15">
         <v>57</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15">
         <v>1903857200</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15">
         <v>63416144</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15">
         <v>19305000</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15">
         <v>10280000</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16">
         <v>2025</v>
@@ -1572,22 +1556,22 @@
       <c r="E16">
         <v>69</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16">
         <v>5876359800</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16">
         <v>197278956</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16">
         <v>8837500</v>
       </c>
-      <c r="I16" s="2">
-        <v>0</v>
+      <c r="I16" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>2025</v>
@@ -1601,22 +1585,22 @@
       <c r="E17">
         <v>63</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17">
         <v>1489350200</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17">
         <v>55620044</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17">
         <v>10050000</v>
       </c>
-      <c r="I17" s="2">
-        <v>0</v>
+      <c r="I17" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>2025</v>
@@ -1630,22 +1614,22 @@
       <c r="E18">
         <v>139</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18">
         <v>5758998700</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18">
         <v>197369304</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18">
         <v>78662650</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18">
         <v>33710850</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19">
         <v>2025</v>
@@ -1659,22 +1643,22 @@
       <c r="E19">
         <v>147</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19">
         <v>6058766000</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19">
         <v>155608500</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19">
         <v>21938975</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19">
         <v>124089550</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B20">
         <v>2025</v>
@@ -1688,22 +1672,22 @@
       <c r="E20">
         <v>156</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20">
         <v>1850945676</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20">
         <v>68543557</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20">
         <v>34532500</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20">
         <v>587200</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21">
         <v>2025</v>
@@ -1717,17 +1701,1815 @@
       <c r="E21">
         <v>127</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21">
         <v>8549514067</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21">
         <v>266064627</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21">
         <v>34675000</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21">
         <v>20172150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22">
+        <v>2025</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>25</v>
+      </c>
+      <c r="F22">
+        <v>84597380000</v>
+      </c>
+      <c r="G22">
+        <v>507584280</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>2025</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>29</v>
+      </c>
+      <c r="E23">
+        <v>29</v>
+      </c>
+      <c r="F23">
+        <v>90460731000</v>
+      </c>
+      <c r="G23">
+        <v>542764386</v>
+      </c>
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>2025</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>27</v>
+      </c>
+      <c r="E24">
+        <v>27</v>
+      </c>
+      <c r="F24">
+        <v>92365037500</v>
+      </c>
+      <c r="G24">
+        <v>553716225</v>
+      </c>
+      <c r="H24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>2025</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>27</v>
+      </c>
+      <c r="E25">
+        <v>27</v>
+      </c>
+      <c r="F25">
+        <v>90556280789</v>
+      </c>
+      <c r="G25">
+        <v>543337685</v>
+      </c>
+      <c r="H25" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <v>2025</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>27</v>
+      </c>
+      <c r="E26">
+        <v>27</v>
+      </c>
+      <c r="F26">
+        <v>94649760333.3333</v>
+      </c>
+      <c r="G26">
+        <v>567898562</v>
+      </c>
+      <c r="H26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>2024</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>45</v>
+      </c>
+      <c r="E27">
+        <v>101</v>
+      </c>
+      <c r="F27">
+        <v>5580094943</v>
+      </c>
+      <c r="G27">
+        <v>134248400</v>
+      </c>
+      <c r="H27">
+        <v>15194250</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>2024</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>31</v>
+      </c>
+      <c r="E28">
+        <v>68</v>
+      </c>
+      <c r="F28">
+        <v>9409654900</v>
+      </c>
+      <c r="G28">
+        <v>221333098</v>
+      </c>
+      <c r="H28">
+        <v>10362500</v>
+      </c>
+      <c r="I28">
+        <v>11750000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>2024</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>132</v>
+      </c>
+      <c r="E29">
+        <v>337</v>
+      </c>
+      <c r="F29">
+        <v>18104076314</v>
+      </c>
+      <c r="G29">
+        <v>523471327</v>
+      </c>
+      <c r="H29">
+        <v>154787925</v>
+      </c>
+      <c r="I29">
+        <v>11000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>2024</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>99</v>
+      </c>
+      <c r="E30">
+        <v>190</v>
+      </c>
+      <c r="F30">
+        <v>12964571565</v>
+      </c>
+      <c r="G30">
+        <v>410174262</v>
+      </c>
+      <c r="H30">
+        <v>164549875</v>
+      </c>
+      <c r="I30">
+        <v>80509750</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>2024</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>179</v>
+      </c>
+      <c r="E31">
+        <v>270</v>
+      </c>
+      <c r="F31">
+        <v>15958592538</v>
+      </c>
+      <c r="G31">
+        <v>493054992</v>
+      </c>
+      <c r="H31">
+        <v>232753925</v>
+      </c>
+      <c r="I31">
+        <v>157694000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>2024</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>127</v>
+      </c>
+      <c r="E32">
+        <v>228</v>
+      </c>
+      <c r="F32">
+        <v>16865160870</v>
+      </c>
+      <c r="G32">
+        <v>926910968</v>
+      </c>
+      <c r="H32">
+        <v>212333900</v>
+      </c>
+      <c r="I32">
+        <v>264544050</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>2024</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>160</v>
+      </c>
+      <c r="E33">
+        <v>278</v>
+      </c>
+      <c r="F33">
+        <v>20141865500</v>
+      </c>
+      <c r="G33">
+        <v>711510066</v>
+      </c>
+      <c r="H33">
+        <v>327691345</v>
+      </c>
+      <c r="I33">
+        <v>96000000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>2024</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34">
+        <v>177</v>
+      </c>
+      <c r="E34">
+        <v>312</v>
+      </c>
+      <c r="F34">
+        <v>8029079712</v>
+      </c>
+      <c r="G34">
+        <v>272053895</v>
+      </c>
+      <c r="H34">
+        <v>101302875</v>
+      </c>
+      <c r="I34">
+        <v>33500000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35">
+        <v>2024</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>167</v>
+      </c>
+      <c r="E35">
+        <v>410</v>
+      </c>
+      <c r="F35">
+        <v>14348755516</v>
+      </c>
+      <c r="G35">
+        <v>524375946</v>
+      </c>
+      <c r="H35">
+        <v>248031675</v>
+      </c>
+      <c r="I35">
+        <v>207185000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36">
+        <v>2024</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>148</v>
+      </c>
+      <c r="E36">
+        <v>282</v>
+      </c>
+      <c r="F36">
+        <v>23882551878</v>
+      </c>
+      <c r="G36">
+        <v>735850498</v>
+      </c>
+      <c r="H36">
+        <v>130744750</v>
+      </c>
+      <c r="I36">
+        <v>76010500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37">
+        <v>2024</v>
+      </c>
+      <c r="C37">
+        <v>11</v>
+      </c>
+      <c r="D37">
+        <v>189</v>
+      </c>
+      <c r="E37">
+        <v>319</v>
+      </c>
+      <c r="F37">
+        <v>24102866050</v>
+      </c>
+      <c r="G37">
+        <v>727732756</v>
+      </c>
+      <c r="H37">
+        <v>261969294</v>
+      </c>
+      <c r="I37">
+        <v>180667500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38">
+        <v>2024</v>
+      </c>
+      <c r="C38">
+        <v>12</v>
+      </c>
+      <c r="D38">
+        <v>211</v>
+      </c>
+      <c r="E38">
+        <v>374</v>
+      </c>
+      <c r="F38">
+        <v>35027813523</v>
+      </c>
+      <c r="G38">
+        <v>1181743531</v>
+      </c>
+      <c r="H38">
+        <v>556764488</v>
+      </c>
+      <c r="I38">
+        <v>338159287.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39">
+        <v>2024</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>54</v>
+      </c>
+      <c r="E39">
+        <v>94</v>
+      </c>
+      <c r="F39">
+        <v>6965037516</v>
+      </c>
+      <c r="G39">
+        <v>198921974</v>
+      </c>
+      <c r="H39">
+        <v>60957700</v>
+      </c>
+      <c r="I39">
+        <v>119515400</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40">
+        <v>2024</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>37</v>
+      </c>
+      <c r="E40">
+        <v>87</v>
+      </c>
+      <c r="F40">
+        <v>9277346949</v>
+      </c>
+      <c r="G40">
+        <v>291932600</v>
+      </c>
+      <c r="H40">
+        <v>86328125</v>
+      </c>
+      <c r="I40">
+        <v>173044250</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41">
+        <v>2024</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>125</v>
+      </c>
+      <c r="E41">
+        <v>186</v>
+      </c>
+      <c r="F41">
+        <v>26274584918</v>
+      </c>
+      <c r="G41">
+        <v>800152317</v>
+      </c>
+      <c r="H41">
+        <v>305311025</v>
+      </c>
+      <c r="I41">
+        <v>642912050</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42">
+        <v>2024</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>102</v>
+      </c>
+      <c r="E42">
+        <v>128</v>
+      </c>
+      <c r="F42">
+        <v>38373513177</v>
+      </c>
+      <c r="G42">
+        <v>1381370600</v>
+      </c>
+      <c r="H42">
+        <v>727608525</v>
+      </c>
+      <c r="I42">
+        <v>1411827050</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43">
+        <v>2024</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <v>112</v>
+      </c>
+      <c r="E43">
+        <v>200</v>
+      </c>
+      <c r="F43">
+        <v>125012080070</v>
+      </c>
+      <c r="G43">
+        <v>4849582942</v>
+      </c>
+      <c r="H43">
+        <v>225925725</v>
+      </c>
+      <c r="I43">
+        <v>445851450</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44">
+        <v>2024</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>137</v>
+      </c>
+      <c r="E44">
+        <v>237</v>
+      </c>
+      <c r="F44">
+        <v>36963292430</v>
+      </c>
+      <c r="G44">
+        <v>1262387496</v>
+      </c>
+      <c r="H44">
+        <v>3309489511</v>
+      </c>
+      <c r="I44">
+        <v>6623679021.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45">
+        <v>2024</v>
+      </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <v>140</v>
+      </c>
+      <c r="E45">
+        <v>205</v>
+      </c>
+      <c r="F45">
+        <v>118552240700</v>
+      </c>
+      <c r="G45">
+        <v>4035705279</v>
+      </c>
+      <c r="H45">
+        <v>1034691087.5</v>
+      </c>
+      <c r="I45">
+        <v>1907382175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46">
+        <v>2024</v>
+      </c>
+      <c r="C46">
+        <v>8</v>
+      </c>
+      <c r="D46">
+        <v>128</v>
+      </c>
+      <c r="E46">
+        <v>178</v>
+      </c>
+      <c r="F46">
+        <v>18100630850</v>
+      </c>
+      <c r="G46">
+        <v>596980507</v>
+      </c>
+      <c r="H46">
+        <v>247386000</v>
+      </c>
+      <c r="I46">
+        <v>422772000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47">
+        <v>2024</v>
+      </c>
+      <c r="C47">
+        <v>9</v>
+      </c>
+      <c r="D47">
+        <v>109</v>
+      </c>
+      <c r="E47">
+        <v>120</v>
+      </c>
+      <c r="F47">
+        <v>24459465984</v>
+      </c>
+      <c r="G47">
+        <v>905379538</v>
+      </c>
+      <c r="H47">
+        <v>471087790.725</v>
+      </c>
+      <c r="I47">
+        <v>665363281.45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48">
+        <v>2024</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>101</v>
+      </c>
+      <c r="E48">
+        <v>99</v>
+      </c>
+      <c r="F48">
+        <v>39103682715</v>
+      </c>
+      <c r="G48">
+        <v>1233080759</v>
+      </c>
+      <c r="H48">
+        <v>493328810</v>
+      </c>
+      <c r="I48">
+        <v>925397620</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49">
+        <v>2024</v>
+      </c>
+      <c r="C49">
+        <v>11</v>
+      </c>
+      <c r="D49">
+        <v>86</v>
+      </c>
+      <c r="E49">
+        <v>103</v>
+      </c>
+      <c r="F49">
+        <v>43834442202</v>
+      </c>
+      <c r="G49">
+        <v>1427949828</v>
+      </c>
+      <c r="H49">
+        <v>502755480.475</v>
+      </c>
+      <c r="I49">
+        <v>965260960.95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50">
+        <v>2024</v>
+      </c>
+      <c r="C50">
+        <v>12</v>
+      </c>
+      <c r="D50">
+        <v>126</v>
+      </c>
+      <c r="E50">
+        <v>168</v>
+      </c>
+      <c r="F50">
+        <v>55334036881</v>
+      </c>
+      <c r="G50">
+        <v>1833785010</v>
+      </c>
+      <c r="H50">
+        <v>825963450</v>
+      </c>
+      <c r="I50">
+        <v>1357601900</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51">
+        <v>2024</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>27</v>
+      </c>
+      <c r="E51">
+        <v>52</v>
+      </c>
+      <c r="F51">
+        <v>2362313277</v>
+      </c>
+      <c r="G51">
+        <v>90588016</v>
+      </c>
+      <c r="H51">
+        <v>1675000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52">
+        <v>2024</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>26</v>
+      </c>
+      <c r="E52">
+        <v>58</v>
+      </c>
+      <c r="F52">
+        <v>2388786700</v>
+      </c>
+      <c r="G52">
+        <v>64625734</v>
+      </c>
+      <c r="H52">
+        <v>8625000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53">
+        <v>2024</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>35</v>
+      </c>
+      <c r="E53">
+        <v>60</v>
+      </c>
+      <c r="F53">
+        <v>3022495900</v>
+      </c>
+      <c r="G53">
+        <v>100699918</v>
+      </c>
+      <c r="H53">
+        <v>40925000</v>
+      </c>
+      <c r="I53">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54">
+        <v>2024</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <v>58</v>
+      </c>
+      <c r="E54">
+        <v>77</v>
+      </c>
+      <c r="F54">
+        <v>3666754400</v>
+      </c>
+      <c r="G54">
+        <v>102456488</v>
+      </c>
+      <c r="H54">
+        <v>29908000</v>
+      </c>
+      <c r="I54">
+        <v>88600000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55">
+        <v>2024</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+      <c r="D55">
+        <v>44</v>
+      </c>
+      <c r="E55">
+        <v>200</v>
+      </c>
+      <c r="F55">
+        <v>5433944200</v>
+      </c>
+      <c r="G55">
+        <v>159293664</v>
+      </c>
+      <c r="H55">
+        <v>55747500</v>
+      </c>
+      <c r="I55">
+        <v>14416420</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56">
+        <v>2024</v>
+      </c>
+      <c r="C56">
+        <v>6</v>
+      </c>
+      <c r="D56">
+        <v>39</v>
+      </c>
+      <c r="E56">
+        <v>101</v>
+      </c>
+      <c r="F56">
+        <v>6432600900</v>
+      </c>
+      <c r="G56">
+        <v>219135148</v>
+      </c>
+      <c r="H56">
+        <v>98613000</v>
+      </c>
+      <c r="I56">
+        <v>144543000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57">
+        <v>2024</v>
+      </c>
+      <c r="C57">
+        <v>7</v>
+      </c>
+      <c r="D57">
+        <v>38</v>
+      </c>
+      <c r="E57">
+        <v>84</v>
+      </c>
+      <c r="F57">
+        <v>2738553700</v>
+      </c>
+      <c r="G57">
+        <v>105373682</v>
+      </c>
+      <c r="H57">
+        <v>30497100</v>
+      </c>
+      <c r="I57">
+        <v>5005000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58">
+        <v>2024</v>
+      </c>
+      <c r="C58">
+        <v>8</v>
+      </c>
+      <c r="D58">
+        <v>82</v>
+      </c>
+      <c r="E58">
+        <v>125</v>
+      </c>
+      <c r="F58">
+        <v>2484425825</v>
+      </c>
+      <c r="G58">
+        <v>81222547</v>
+      </c>
+      <c r="H58">
+        <v>46625000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59">
+        <v>2024</v>
+      </c>
+      <c r="C59">
+        <v>9</v>
+      </c>
+      <c r="D59">
+        <v>38</v>
+      </c>
+      <c r="E59">
+        <v>52</v>
+      </c>
+      <c r="F59">
+        <v>1509767000</v>
+      </c>
+      <c r="G59">
+        <v>46632246</v>
+      </c>
+      <c r="H59">
+        <v>11325000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60">
+        <v>2024</v>
+      </c>
+      <c r="C60">
+        <v>10</v>
+      </c>
+      <c r="D60">
+        <v>62</v>
+      </c>
+      <c r="E60">
+        <v>92</v>
+      </c>
+      <c r="F60">
+        <v>7995415755</v>
+      </c>
+      <c r="G60">
+        <v>279083518</v>
+      </c>
+      <c r="H60">
+        <v>112475000</v>
+      </c>
+      <c r="I60">
+        <v>15913050</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61">
+        <v>2024</v>
+      </c>
+      <c r="C61">
+        <v>11</v>
+      </c>
+      <c r="D61">
+        <v>37</v>
+      </c>
+      <c r="E61">
+        <v>66</v>
+      </c>
+      <c r="F61">
+        <v>3319522300</v>
+      </c>
+      <c r="G61">
+        <v>103445179</v>
+      </c>
+      <c r="H61">
+        <v>28861000</v>
+      </c>
+      <c r="I61">
+        <v>62206500</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62">
+        <v>2024</v>
+      </c>
+      <c r="C62">
+        <v>12</v>
+      </c>
+      <c r="D62">
+        <v>53</v>
+      </c>
+      <c r="E62">
+        <v>111</v>
+      </c>
+      <c r="F62">
+        <v>16564513400</v>
+      </c>
+      <c r="G62">
+        <v>588444178</v>
+      </c>
+      <c r="H62">
+        <v>113409850</v>
+      </c>
+      <c r="I62">
+        <v>4300000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63">
+        <v>2024</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>64</v>
+      </c>
+      <c r="E63">
+        <v>107</v>
+      </c>
+      <c r="F63">
+        <v>2466200966</v>
+      </c>
+      <c r="G63">
+        <v>70925354</v>
+      </c>
+      <c r="H63">
+        <v>23219166.65</v>
+      </c>
+      <c r="I63">
+        <v>2833333</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64">
+        <v>2024</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <v>33</v>
+      </c>
+      <c r="E64">
+        <v>49</v>
+      </c>
+      <c r="F64">
+        <v>4595163924</v>
+      </c>
+      <c r="G64">
+        <v>129453480</v>
+      </c>
+      <c r="H64">
+        <v>28062850.6</v>
+      </c>
+      <c r="I64">
+        <v>18761550</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>13</v>
+      </c>
+      <c r="B65">
+        <v>2024</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65">
+        <v>73</v>
+      </c>
+      <c r="E65">
+        <v>93</v>
+      </c>
+      <c r="F65">
+        <v>12050284977</v>
+      </c>
+      <c r="G65">
+        <v>423516700</v>
+      </c>
+      <c r="H65">
+        <v>207977500</v>
+      </c>
+      <c r="I65">
+        <v>364405000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66">
+        <v>2024</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66">
+        <v>69</v>
+      </c>
+      <c r="E66">
+        <v>102</v>
+      </c>
+      <c r="F66">
+        <v>5495591500</v>
+      </c>
+      <c r="G66">
+        <v>189700689</v>
+      </c>
+      <c r="H66">
+        <v>84325500</v>
+      </c>
+      <c r="I66">
+        <v>21683000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67">
+        <v>2024</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
+      </c>
+      <c r="D67">
+        <v>47</v>
+      </c>
+      <c r="E67">
+        <v>73</v>
+      </c>
+      <c r="F67">
+        <v>13595430735</v>
+      </c>
+      <c r="G67">
+        <v>557382724</v>
+      </c>
+      <c r="H67">
+        <v>86853050</v>
+      </c>
+      <c r="I67">
+        <v>137150000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>13</v>
+      </c>
+      <c r="B68">
+        <v>2024</v>
+      </c>
+      <c r="C68">
+        <v>6</v>
+      </c>
+      <c r="D68">
+        <v>87</v>
+      </c>
+      <c r="E68">
+        <v>143</v>
+      </c>
+      <c r="F68">
+        <v>6087453807</v>
+      </c>
+      <c r="G68">
+        <v>238472367</v>
+      </c>
+      <c r="H68">
+        <v>121073957.275</v>
+      </c>
+      <c r="I68">
+        <v>6292000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69">
+        <v>2024</v>
+      </c>
+      <c r="C69">
+        <v>7</v>
+      </c>
+      <c r="D69">
+        <v>73</v>
+      </c>
+      <c r="E69">
+        <v>94</v>
+      </c>
+      <c r="F69">
+        <v>6130696506</v>
+      </c>
+      <c r="G69">
+        <v>185035751</v>
+      </c>
+      <c r="H69">
+        <v>61393888.15</v>
+      </c>
+      <c r="I69">
+        <v>83900000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70">
+        <v>2024</v>
+      </c>
+      <c r="C70">
+        <v>8</v>
+      </c>
+      <c r="D70">
+        <v>88</v>
+      </c>
+      <c r="E70">
+        <v>150</v>
+      </c>
+      <c r="F70">
+        <v>80004125200</v>
+      </c>
+      <c r="G70">
+        <v>4282324724</v>
+      </c>
+      <c r="H70">
+        <v>115267150</v>
+      </c>
+      <c r="I70">
+        <v>195129976</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71">
+        <v>2024</v>
+      </c>
+      <c r="C71">
+        <v>9</v>
+      </c>
+      <c r="D71">
+        <v>68</v>
+      </c>
+      <c r="E71">
+        <v>106</v>
+      </c>
+      <c r="F71">
+        <v>5545256850</v>
+      </c>
+      <c r="G71">
+        <v>180131064</v>
+      </c>
+      <c r="H71">
+        <v>61283883.75</v>
+      </c>
+      <c r="I71">
+        <v>3214513541</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72">
+        <v>2024</v>
+      </c>
+      <c r="C72">
+        <v>10</v>
+      </c>
+      <c r="D72">
+        <v>81</v>
+      </c>
+      <c r="E72">
+        <v>165</v>
+      </c>
+      <c r="F72">
+        <v>11577980870</v>
+      </c>
+      <c r="G72">
+        <v>392973988</v>
+      </c>
+      <c r="H72">
+        <v>155583956.15</v>
+      </c>
+      <c r="I72">
+        <v>238661728</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>13</v>
+      </c>
+      <c r="B73">
+        <v>2024</v>
+      </c>
+      <c r="C73">
+        <v>11</v>
+      </c>
+      <c r="D73">
+        <v>88</v>
+      </c>
+      <c r="E73">
+        <v>447</v>
+      </c>
+      <c r="F73">
+        <v>14326419985</v>
+      </c>
+      <c r="G73">
+        <v>455183611</v>
+      </c>
+      <c r="H73">
+        <v>180550175</v>
+      </c>
+      <c r="I73">
+        <v>118392100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74">
+        <v>2024</v>
+      </c>
+      <c r="C74">
+        <v>12</v>
+      </c>
+      <c r="D74">
+        <v>87</v>
+      </c>
+      <c r="E74">
+        <v>170</v>
+      </c>
+      <c r="F74">
+        <v>7043961226</v>
+      </c>
+      <c r="G74">
+        <v>236105571</v>
+      </c>
+      <c r="H74">
+        <v>318103007.5</v>
+      </c>
+      <c r="I74">
+        <v>21000000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75">
+        <v>2024</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>13</v>
+      </c>
+      <c r="E75">
+        <v>3534</v>
+      </c>
+      <c r="F75">
+        <v>70752784550</v>
+      </c>
+      <c r="G75">
+        <v>424516707</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
+        <v>14</v>
+      </c>
+      <c r="B76">
+        <v>2024</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76">
+        <v>12</v>
+      </c>
+      <c r="E76">
+        <v>3686</v>
+      </c>
+      <c r="F76">
+        <v>67019040500</v>
+      </c>
+      <c r="G76">
+        <v>402114243</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77">
+        <v>2024</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77">
+        <v>13</v>
+      </c>
+      <c r="E77">
+        <v>4025</v>
+      </c>
+      <c r="F77">
+        <v>83789270000</v>
+      </c>
+      <c r="G77">
+        <v>502735620</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78">
+        <v>2024</v>
+      </c>
+      <c r="C78">
+        <v>4</v>
+      </c>
+      <c r="D78">
+        <v>12</v>
+      </c>
+      <c r="E78">
+        <v>3356</v>
+      </c>
+      <c r="F78">
+        <v>79684721575</v>
+      </c>
+      <c r="G78">
+        <v>478108329</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79">
+        <v>2024</v>
+      </c>
+      <c r="C79">
+        <v>5</v>
+      </c>
+      <c r="D79">
+        <v>16</v>
+      </c>
+      <c r="E79">
+        <v>4093</v>
+      </c>
+      <c r="F79">
+        <v>92153082000</v>
+      </c>
+      <c r="G79">
+        <v>552918492</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80">
+        <v>2024</v>
+      </c>
+      <c r="C80">
+        <v>6</v>
+      </c>
+      <c r="D80">
+        <v>16</v>
+      </c>
+      <c r="E80">
+        <v>3904</v>
+      </c>
+      <c r="F80">
+        <v>75171493333.3333</v>
+      </c>
+      <c r="G80">
+        <v>451028960</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" t="s">
+        <v>14</v>
+      </c>
+      <c r="B81">
+        <v>2024</v>
+      </c>
+      <c r="C81">
+        <v>7</v>
+      </c>
+      <c r="D81">
+        <v>22</v>
+      </c>
+      <c r="E81">
+        <v>5173</v>
+      </c>
+      <c r="F81">
+        <v>95341452166.6667</v>
+      </c>
+      <c r="G81">
+        <v>572048713</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
+        <v>14</v>
+      </c>
+      <c r="B82">
+        <v>2024</v>
+      </c>
+      <c r="C82">
+        <v>8</v>
+      </c>
+      <c r="D82">
+        <v>22</v>
+      </c>
+      <c r="E82">
+        <v>4271</v>
+      </c>
+      <c r="F82">
+        <v>104052091500</v>
+      </c>
+      <c r="G82">
+        <v>624312549</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
+        <v>14</v>
+      </c>
+      <c r="B83">
+        <v>2024</v>
+      </c>
+      <c r="C83">
+        <v>9</v>
+      </c>
+      <c r="D83">
+        <v>17</v>
+      </c>
+      <c r="E83">
+        <v>4214</v>
+      </c>
+      <c r="F83">
+        <v>78719227000</v>
+      </c>
+      <c r="G83">
+        <v>472315362</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>14</v>
+      </c>
+      <c r="B84">
+        <v>2024</v>
+      </c>
+      <c r="C84">
+        <v>10</v>
+      </c>
+      <c r="D84">
+        <v>23</v>
+      </c>
+      <c r="E84">
+        <v>5069</v>
+      </c>
+      <c r="F84">
+        <v>96744232166.6667</v>
+      </c>
+      <c r="G84">
+        <v>580465393</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>14</v>
+      </c>
+      <c r="B85">
+        <v>2024</v>
+      </c>
+      <c r="C85">
+        <v>11</v>
+      </c>
+      <c r="D85">
+        <v>21</v>
+      </c>
+      <c r="E85">
+        <v>3236</v>
+      </c>
+      <c r="F85">
+        <v>85778702666.6667</v>
+      </c>
+      <c r="G85">
+        <v>514672216</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>14</v>
+      </c>
+      <c r="B86">
+        <v>2024</v>
+      </c>
+      <c r="C86">
+        <v>12</v>
+      </c>
+      <c r="D86">
+        <v>22</v>
+      </c>
+      <c r="E86">
+        <v>2627</v>
+      </c>
+      <c r="F86">
+        <v>82119849000</v>
+      </c>
+      <c r="G86">
+        <v>495989094</v>
       </c>
     </row>
   </sheetData>
@@ -1739,19 +3521,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="3" max="5" width="19.4545454545455" customWidth="1"/>
-    <col min="6" max="6" width="21.0909090909091" customWidth="1"/>
-    <col min="7" max="8" width="17.1818181818182"/>
-    <col min="9" max="10" width="18.3636363636364"/>
+    <col min="1" max="1" width="21.7272727272727" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1762,28 +3540,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1793,157 +3571,317 @@
       <c r="B2">
         <v>2025</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>36720000000</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>71660000000</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>121320000000</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>202200000000</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>1577200000</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>3154400000</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2">
         <v>5231600000</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2">
         <v>7886000000</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>2025</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>22065000000</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>132390000000</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>264780000000</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>441300000000</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>1556950000</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <v>6316800000</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3">
         <v>12633600000</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3">
         <v>21056000000</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>2025</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>25350000000</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>76050000000</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>101400000000</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <v>169000000000</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>1304400000</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4">
         <v>2934900000</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4">
         <v>3913200000</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4">
         <v>6522000000</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>2025</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>5800000000</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>17400000000</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>34800000000</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <v>58000000000</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>270500000</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <v>811500000</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5">
         <v>1623000000</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5">
         <v>2705000000</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>2025</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>214772000000</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>429544000000</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>859089000000</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6">
         <v>1073861000000</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>1067000000</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6">
         <v>2133000000</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6">
         <v>4266000000</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6">
         <v>5333000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>2024</v>
+      </c>
+      <c r="C7">
+        <v>15225896736.4</v>
+      </c>
+      <c r="D7">
+        <v>45677690209.2</v>
+      </c>
+      <c r="E7">
+        <v>91355380418.4</v>
+      </c>
+      <c r="F7">
+        <v>152258967364</v>
+      </c>
+      <c r="G7">
+        <v>750986605</v>
+      </c>
+      <c r="H7">
+        <v>2252959814</v>
+      </c>
+      <c r="I7">
+        <v>4505919629</v>
+      </c>
+      <c r="J7">
+        <v>7509866048</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>2024</v>
+      </c>
+      <c r="C8">
+        <v>124876257896.4</v>
+      </c>
+      <c r="D8">
+        <v>208127096494</v>
+      </c>
+      <c r="E8">
+        <v>333003354390.4</v>
+      </c>
+      <c r="F8">
+        <v>416254192988</v>
+      </c>
+      <c r="G8">
+        <v>8422271242</v>
+      </c>
+      <c r="H8">
+        <v>16844542484</v>
+      </c>
+      <c r="I8">
+        <v>18950110294.5</v>
+      </c>
+      <c r="J8">
+        <v>21055678105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>2024</v>
+      </c>
+      <c r="C9">
+        <v>3907980162.3</v>
+      </c>
+      <c r="D9">
+        <v>11723940486.9</v>
+      </c>
+      <c r="E9">
+        <v>23447880973.8</v>
+      </c>
+      <c r="F9">
+        <v>39079801623</v>
+      </c>
+      <c r="G9">
+        <v>270423730</v>
+      </c>
+      <c r="H9">
+        <v>811271189</v>
+      </c>
+      <c r="I9">
+        <v>1622542379</v>
+      </c>
+      <c r="J9">
+        <v>2704237298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>2024</v>
+      </c>
+      <c r="C10">
+        <v>10252103802.5</v>
+      </c>
+      <c r="D10">
+        <v>30756311407.5</v>
+      </c>
+      <c r="E10">
+        <v>61512622815</v>
+      </c>
+      <c r="F10">
+        <v>102521038025</v>
+      </c>
+      <c r="G10">
+        <v>347667738.1</v>
+      </c>
+      <c r="H10">
+        <v>1043003214.3</v>
+      </c>
+      <c r="I10">
+        <v>2433674166.7</v>
+      </c>
+      <c r="J10">
+        <v>3476677381</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>2024</v>
+      </c>
+      <c r="C11">
+        <v>64000000000</v>
+      </c>
+      <c r="D11">
+        <v>192000000000</v>
+      </c>
+      <c r="E11">
+        <v>448000000000</v>
+      </c>
+      <c r="F11">
+        <v>640000000000</v>
+      </c>
+      <c r="G11">
+        <v>386054116.8</v>
+      </c>
+      <c r="H11">
+        <v>1158162350.4</v>
+      </c>
+      <c r="I11">
+        <v>2702378817.6</v>
+      </c>
+      <c r="J11">
+        <v>3860541168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>